<commit_message>
Increase height of test case "Rows of a Worksheet" in RowCollection  for easier visual comparison.
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Examples/Rows/RowCollection.xlsx
+++ b/ClosedXML.Tests/Resource/Examples/Rows/RowCollection.xlsx
@@ -494,19 +494,19 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" s="2" customFormat="1" ht="15" customHeight="1"/>
-    <x:row r="2" s="2" customFormat="1" ht="15" customHeight="1"/>
-    <x:row r="3" ht="15" customHeight="1"/>
-    <x:row r="4" s="3" customFormat="1" ht="15" customHeight="1"/>
-    <x:row r="5" s="3" customFormat="1" ht="15" customHeight="1"/>
-    <x:row r="6" ht="15" customHeight="1"/>
-    <x:row r="7" s="4" customFormat="1" ht="15" customHeight="1"/>
-    <x:row r="8" s="4" customFormat="1" ht="15" customHeight="1"/>
-    <x:row r="9" ht="15" customHeight="1"/>
-    <x:row r="10" s="4" customFormat="1" ht="15" customHeight="1"/>
-    <x:row r="11" s="4" customFormat="1" ht="15" customHeight="1"/>
-    <x:row r="12" ht="15" customHeight="1"/>
-    <x:row r="13" s="5" customFormat="1" ht="15" customHeight="1"/>
+    <x:row r="1" s="2" customFormat="1" ht="30" customHeight="1"/>
+    <x:row r="2" s="2" customFormat="1" ht="30" customHeight="1"/>
+    <x:row r="3" ht="30" customHeight="1"/>
+    <x:row r="4" s="3" customFormat="1" ht="30" customHeight="1"/>
+    <x:row r="5" s="3" customFormat="1" ht="30" customHeight="1"/>
+    <x:row r="6" ht="30" customHeight="1"/>
+    <x:row r="7" s="4" customFormat="1" ht="30" customHeight="1"/>
+    <x:row r="8" s="4" customFormat="1" ht="30" customHeight="1"/>
+    <x:row r="9" ht="30" customHeight="1"/>
+    <x:row r="10" s="4" customFormat="1" ht="30" customHeight="1"/>
+    <x:row r="11" s="4" customFormat="1" ht="30" customHeight="1"/>
+    <x:row r="12" ht="30" customHeight="1"/>
+    <x:row r="13" s="5" customFormat="1" ht="30" customHeight="1"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>